<commit_message>
PowerBI Report + some more work on saving the date
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -14,9 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Name</t>
+  </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Date&amp;Time</t>
   </si>
 </sst>
 </file>
@@ -348,25 +354,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1">
-        <v>1137</v>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2">
-        <v>1603</v>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <v>1907</v>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New writing to excel method implemented (wayy better) and formatting of the columns + creating a table style dynamically, according to the number of lots selected by the user.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,64 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
-  <si>
-    <t>Lot0</t>
-  </si>
-  <si>
-    <t>LIBER</t>
-  </si>
-  <si>
-    <t>Lot1</t>
-  </si>
-  <si>
-    <t>Lot2</t>
-  </si>
-  <si>
-    <t>Lot3</t>
-  </si>
-  <si>
-    <t>OCUPAT</t>
-  </si>
-  <si>
-    <t>03-16-2021 22:38:21</t>
-  </si>
-  <si>
-    <t>Lot4</t>
-  </si>
-  <si>
-    <t>Lot5</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -77,14 +47,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E14" headerRowCount="1">
+  <autoFilter ref="A1:E14"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Lot"/>
+    <tableColumn id="2" name="Status"/>
+    <tableColumn id="3" name="Date&amp;Time"/>
+    <tableColumn id="4" name="BusySpaces"/>
+    <tableColumn id="5" name="FreeSpaces"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,116 +422,325 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>22</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Lot</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Date&amp;Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>BusySpaces</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>FreeSpaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Lot0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>OCUPAT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>03-29-2021 22:01:21</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Lot1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Lot2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Lot3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Lot4</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Lot5</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Lot6</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Lot7</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Lot8</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Lot9</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Lot10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Lot11</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Lot12</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New selection method in testing. Last known working update.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -125,14 +125,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E14" headerRowCount="1">
-  <autoFilter ref="A1:E14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E1" headerRowCount="1">
+  <autoFilter ref="A1:E1"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Lot"/>
-    <tableColumn id="2" name="Status"/>
-    <tableColumn id="3" name="Date&amp;Time"/>
-    <tableColumn id="4" name="BusySpaces"/>
-    <tableColumn id="5" name="FreeSpaces"/>
+    <tableColumn id="1" name="None"/>
+    <tableColumn id="2" name="None"/>
+    <tableColumn id="3" name="None"/>
+    <tableColumn id="4" name="None"/>
+    <tableColumn id="5" name="None"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -427,317 +427,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Lot</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Date&amp;Time</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>BusySpaces</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>FreeSpaces</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Lot0</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>OCUPAT</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>03-29-2021 22:01:21</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Lot1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Lot2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Lot3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Lot4</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Lot5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Lot6</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Lot7</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Lot8</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Lot9</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Lot10</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Lot11</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Lot12</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>LIBER</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" t="n">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
New selection method implemente. Now worrking on parsing compatibility to WhitePixel Counter.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -125,14 +125,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E1" headerRowCount="1">
-  <autoFilter ref="A1:E1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E2" headerRowCount="1">
+  <autoFilter ref="A1:E2"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="None"/>
-    <tableColumn id="2" name="None"/>
-    <tableColumn id="3" name="None"/>
-    <tableColumn id="4" name="None"/>
-    <tableColumn id="5" name="None"/>
+    <tableColumn id="1" name="Lot"/>
+    <tableColumn id="2" name="Status"/>
+    <tableColumn id="3" name="Date&amp;Time"/>
+    <tableColumn id="4" name="BusySpaces"/>
+    <tableColumn id="5" name="FreeSpaces"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -427,14 +427,53 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Lot</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Date&amp;Time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>BusySpaces</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>FreeSpaces</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
FIltering done, processing part not working properly..
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -125,8 +125,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E2" headerRowCount="1">
-  <autoFilter ref="A1:E2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E4" headerRowCount="1">
+  <autoFilter ref="A1:E4"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Lot"/>
     <tableColumn id="2" name="Status"/>
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,14 +463,72 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Lot0</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>OCUPAT</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>04-08-2021 23:56:41</t>
+        </is>
+      </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>25</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Lot1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>OCUPAT</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>04-08-2021 23:56:41</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Lot2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>OCUPAT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>04-08-2021 23:56:41</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Processing part done. Increased accuracy. Cleaned project files.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -470,19 +470,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>OCUPAT</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>04-08-2021 23:56:41</t>
-        </is>
+          <t>LIBER</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -498,14 +496,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>04-08-2021 23:56:41</t>
+          <t>04-24-2021 16:56:56</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -521,14 +519,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>04-08-2021 23:56:41</t>
+          <t>04-24-2021 16:56:56</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>